<commit_message>
Added all files and updated test plan
</commit_message>
<xml_diff>
--- a/Documentation/TestFall.xlsx
+++ b/Documentation/TestFall.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local\Peter\Testning\SecuremeTesting@fendraq\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F137921F-7692-4052-BE30-B17AC1BCA725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8C21DC-8537-4946-9DD0-1349AA9C4A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" firstSheet="5" activeTab="7" xr2:uid="{A195DD68-4712-4E96-A3AE-C1124A7416DB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kravspecifikationer" sheetId="2" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="167">
   <si>
     <t>Test-ID</t>
   </si>
@@ -236,9 +235,6 @@
     <t>-          API:er returnerar rätt statuskoder</t>
   </si>
   <si>
-    <t>Testningen omfattar ärendeformulär, mejl -, och ärendehantering, nya användare samt chattfunktionalitet.</t>
-  </si>
-  <si>
     <t> Kan jag testa?</t>
   </si>
   <si>
@@ -380,18 +376,6 @@
     <t>Unit - Backend</t>
   </si>
   <si>
-    <t>Säkerställer att konstruktorn i modellklassen Message sätter värden korrekt</t>
-  </si>
-  <si>
-    <t>Konstruktorn returnerar rätt värden och datatyper</t>
-  </si>
-  <si>
-    <t>Verifiera att konstruktorn i modellklassen User sätter värden korrekt</t>
-  </si>
-  <si>
-    <t>Verifiera att konstruktorn i modellklassen Case sätter värden korrekt</t>
-  </si>
-  <si>
     <t>API - Endpoint</t>
   </si>
   <si>
@@ -516,6 +500,39 @@
   </si>
   <si>
     <t>Verifiera att menyn byter vy</t>
+  </si>
+  <si>
+    <t>Verifiera att konstruktorn i modellklassen User sätter alla fält korrekt</t>
+  </si>
+  <si>
+    <t>Verifiera att konstruktorn i modellklassen Case sätter alla fält korrekt</t>
+  </si>
+  <si>
+    <t>Säkerställer att konstruktorn i modellklassen Message sätter alla fält korrekt</t>
+  </si>
+  <si>
+    <t>Konstruktorn returnerar objekt med korrekta värden</t>
+  </si>
+  <si>
+    <t>EX: Testar med både null och giltig input</t>
+  </si>
+  <si>
+    <t>HTTP 200 + JSON-array med rätt struktur</t>
+  </si>
+  <si>
+    <t>Mockdata</t>
+  </si>
+  <si>
+    <t>Fälten validerar korrekt input och visar felmeddelanden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Använde: </t>
+  </si>
+  <si>
+    <t>-          om API för login i backend är uppbyggd för att kunna hantera vidare påbyggnad för login i frontend</t>
+  </si>
+  <si>
+    <t>Testningen omfattar ärendeformulär, mejl -, och ärendehantering, nya användare samt chattfunktionalitet. (Login - API i backend)</t>
   </si>
 </sst>
 </file>
@@ -590,7 +607,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -650,11 +667,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -675,13 +707,16 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -970,7 +1005,6 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:A8"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1026,11 +1060,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5464F935-DEAA-4EF7-8B39-9358828D74A1}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A9"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1439,7 +1472,6 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1842,13 +1874,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DAC0F83-9806-4801-90A6-2FE0AA568BAD}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2033,7 +2064,7 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B17" s="3"/>
@@ -2044,8 +2075,8 @@
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
-        <v>53</v>
+      <c r="A18" s="11" t="s">
+        <v>165</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2055,8 +2086,8 @@
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
-        <v>66</v>
+      <c r="A19" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2066,7 +2097,9 @@
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
+      <c r="A20" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2244,6 +2277,15 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2254,11 +2296,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC31A750-71E8-4741-BD79-BC2E7283B985}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2276,7 +2317,7 @@
     </row>
     <row r="2" spans="1:7" ht="22" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>166</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2287,7 +2328,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2631,9 +2672,8 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2651,7 +2691,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2662,7 +2702,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2673,7 +2713,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3010,7 +3050,6 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3029,7 +3068,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -3040,7 +3079,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3051,7 +3090,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3384,13 +3423,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
-    </sheetView>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="1">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3408,16 +3443,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -3434,41 +3469,43 @@
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -3476,20 +3513,20 @@
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -3497,16 +3534,16 @@
     </row>
     <row r="5" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -3516,7 +3553,7 @@
     </row>
     <row r="6" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3529,7 +3566,7 @@
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3542,7 +3579,7 @@
     </row>
     <row r="8" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3555,7 +3592,7 @@
     </row>
     <row r="9" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -3568,7 +3605,7 @@
     </row>
     <row r="10" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3581,7 +3618,7 @@
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -3594,7 +3631,7 @@
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -3607,38 +3644,42 @@
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>161</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="3" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -3647,16 +3688,16 @@
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -3666,16 +3707,16 @@
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -3685,16 +3726,16 @@
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -3704,16 +3745,16 @@
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -3723,19 +3764,19 @@
     </row>
     <row r="19" spans="1:9" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -3744,19 +3785,19 @@
     </row>
     <row r="20" spans="1:9" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -3765,19 +3806,19 @@
     </row>
     <row r="21" spans="1:9" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -3786,16 +3827,16 @@
     </row>
     <row r="22" spans="1:9" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -3805,19 +3846,19 @@
     </row>
     <row r="23" spans="1:9" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -3826,16 +3867,16 @@
     </row>
     <row r="24" spans="1:9" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -3845,19 +3886,19 @@
     </row>
     <row r="25" spans="1:9" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -3866,19 +3907,19 @@
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -3887,16 +3928,16 @@
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -3906,31 +3947,35 @@
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="I28" s="3" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="29" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -3940,17 +3985,17 @@
     </row>
     <row r="30" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -3959,17 +4004,17 @@
     </row>
     <row r="31" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -3978,17 +4023,17 @@
     </row>
     <row r="32" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -3997,14 +4042,14 @@
     </row>
     <row r="33" spans="1:9" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -4014,14 +4059,14 @@
     </row>
     <row r="34" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -4031,14 +4076,14 @@
     </row>
     <row r="35" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -4048,10 +4093,10 @@
     </row>
     <row r="36" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -4063,10 +4108,10 @@
     </row>
     <row r="37" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -4078,10 +4123,10 @@
     </row>
     <row r="38" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -4093,10 +4138,10 @@
     </row>
     <row r="39" spans="1:9" s="5" customFormat="1" ht="10.5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>

</xml_diff>